<commit_message>
Fixing failures - duplicateEmail sign up got ignored Changing available language
</commit_message>
<xml_diff>
--- a/resources/testdata/SignUpTestCases.xlsx
+++ b/resources/testdata/SignUpTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>TCID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>language</t>
   </si>
   <si>
-    <t>DUTCH</t>
-  </si>
-  <si>
     <t>cityName</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>ensimautotest@outlook.com</t>
+  </si>
+  <si>
+    <t>English (US)</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -467,21 +470,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -497,7 +500,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +508,7 @@
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -522,7 +526,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,20 +534,21 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -551,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -562,12 +567,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>